<commit_message>
Updated file to correct mistake
Corrected - bing_defrebs and other_defrebs
</commit_message>
<xml_diff>
--- a/Bing2022-2023.xlsx
+++ b/Bing2022-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6673BD47-33CB-4493-B6F5-C9AE55685EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D91B6BD-CC9F-41D9-89CE-6416B481984D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{91354573-5B96-4EF4-AC88-42AB5826D78B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{91354573-5B96-4EF4-AC88-42AB5826D78B}"/>
   </bookViews>
   <sheets>
     <sheet name="2022-2023" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
   <si>
     <t>W</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>other_ftp</t>
+  </si>
+  <si>
+    <t>bing_defrebs</t>
+  </si>
+  <si>
+    <t>other_defrebs</t>
   </si>
 </sst>
 </file>
@@ -631,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE028C3E-B7FD-4500-88B9-B57AF0577A84}">
   <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,10 +703,10 @@
         <v>37</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>40</v>

</xml_diff>